<commit_message>
Imported true and measured values
</commit_message>
<xml_diff>
--- a/Measurement.xlsx
+++ b/Measurement.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="19008" windowHeight="7332"/>
+    <workbookView xWindow="100" yWindow="40" windowWidth="19000" windowHeight="7340"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
     <sheet name="True values" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -488,14 +493,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="2" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -509,7 +514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -531,7 +536,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -545,7 +550,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -559,7 +564,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -573,7 +578,7 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>8</v>
       </c>
@@ -587,7 +592,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>10</v>
       </c>
@@ -601,7 +606,7 @@
         <v>5.34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>12</v>
       </c>
@@ -615,7 +620,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>14</v>
       </c>
@@ -629,7 +634,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>16</v>
       </c>
@@ -643,7 +648,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>18</v>
       </c>
@@ -657,7 +662,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>20</v>
       </c>
@@ -671,7 +676,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>22</v>
       </c>
@@ -685,7 +690,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>24</v>
       </c>
@@ -699,7 +704,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>26</v>
       </c>
@@ -713,7 +718,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>28</v>
       </c>
@@ -727,7 +732,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="2">
         <v>30</v>
       </c>
@@ -741,7 +746,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>32</v>
       </c>
@@ -755,7 +760,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="2">
         <v>34</v>
       </c>
@@ -769,7 +774,7 @@
         <v>5.57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>36</v>
       </c>
@@ -783,7 +788,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="2">
         <v>38</v>
       </c>
@@ -797,7 +802,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>40</v>
       </c>
@@ -811,7 +816,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="2">
         <v>42</v>
       </c>
@@ -825,7 +830,7 @@
         <v>4.96</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="2">
         <v>44</v>
       </c>
@@ -839,7 +844,7 @@
         <v>5.59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="2">
         <v>46</v>
       </c>
@@ -853,7 +858,7 @@
         <v>5.81</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="2">
         <v>48</v>
       </c>
@@ -869,6 +874,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -880,9 +890,9 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -916,7 +926,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -933,7 +943,7 @@
         <v>2.49714299461015</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -950,7 +960,7 @@
         <v>2.5467842284251501</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>6</v>
       </c>
@@ -967,7 +977,7 @@
         <v>2.7566160805757698</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>8</v>
       </c>
@@ -984,7 +994,7 @@
         <v>2.58276193994317</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="4">
         <v>10</v>
       </c>
@@ -1001,7 +1011,7 @@
         <v>2.5512826227234799</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
         <v>12</v>
       </c>
@@ -1018,7 +1028,7 @@
         <v>2.60807652804721</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -1035,7 +1045,7 @@
         <v>2.7040520027111499</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
         <v>16</v>
       </c>
@@ -1052,7 +1062,7 @@
         <v>2.8027116093405899</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <v>18</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>2.6154089537290099</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>2.7788031087440501</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
         <v>22</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>2.7957979044002199</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
         <v>24</v>
       </c>
@@ -1120,7 +1130,7 @@
         <v>2.6591179233922801</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="4">
         <v>26</v>
       </c>
@@ -1137,7 +1147,7 @@
         <v>2.50038756002894</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>28</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>2.5638714911835998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="4">
         <v>30</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>2.3910245849346201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="4">
         <v>32</v>
       </c>
@@ -1188,7 +1198,7 @@
         <v>2.2626183451853601</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="4">
         <v>34</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>2.1979689924762602</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="4">
         <v>36</v>
       </c>
@@ -1222,7 +1232,7 @@
         <v>2.22556908557452</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="4">
         <v>38</v>
       </c>
@@ -1239,7 +1249,7 @@
         <v>2.37255823321546</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="4">
         <v>40</v>
       </c>
@@ -1256,7 +1266,7 @@
         <v>2.4002172520151999</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="4">
         <v>42</v>
       </c>
@@ -1273,7 +1283,7 @@
         <v>2.4223265079674698</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="4">
         <v>44</v>
       </c>
@@ -1290,7 +1300,7 @@
         <v>2.2567589439446198</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="4">
         <v>46</v>
       </c>
@@ -1307,7 +1317,7 @@
         <v>2.2092019285448199</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="4">
         <v>48</v>
       </c>
@@ -1326,7 +1336,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1336,8 +1351,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>